<commit_message>
Implemented the first skeletton classes and changed the tasks excel to hours per person
</commit_message>
<xml_diff>
--- a/01_ProjectPlanning/Tasks/Tasks.xlsx
+++ b/01_ProjectPlanning/Tasks/Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\SYP\if.05.61_01-project-repository\01_ProjectPlanning\Tasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B63E074B-8C1C-408B-955C-45177FED56A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42AB5E7-EA83-4DFD-A63A-B768BF042C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DD3696FE-717E-4025-B52C-339B2E8794CF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{DD3696FE-717E-4025-B52C-339B2E8794CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -54,9 +54,6 @@
     <t>Responsible</t>
   </si>
   <si>
-    <t>Iplement classes as good and easy as possible</t>
-  </si>
-  <si>
     <t>Implement the virus with all ist math and physiks</t>
   </si>
   <si>
@@ -73,6 +70,9 @@
   </si>
   <si>
     <t>Implement the complex and math-heavy methods</t>
+  </si>
+  <si>
+    <t>Implement calsses according to UML-class diagram without virus</t>
   </si>
 </sst>
 </file>
@@ -462,16 +462,16 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="118.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.42578125" customWidth="1"/>
+    <col min="1" max="1" width="118.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -491,106 +491,106 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="3">
         <v>6</v>
-      </c>
-      <c r="B2" s="3">
-        <v>3</v>
       </c>
       <c r="C2" s="3">
         <f>B2</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C3" s="3">
         <f t="shared" ref="C3:C8" si="0">B3</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3">
         <v>12</v>
-      </c>
-      <c r="B4" s="3">
-        <v>5</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="3">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="3">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>

</xml_diff>

<commit_message>
Changed the effort sheet and talked about our results and remainings
</commit_message>
<xml_diff>
--- a/01_ProjectPlanning/Tasks/Tasks.xlsx
+++ b/01_ProjectPlanning/Tasks/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\SYP\if.05.61_01-project-repository\01_ProjectPlanning\Tasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42AB5E7-EA83-4DFD-A63A-B768BF042C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D8DF41-02E5-44B4-AC8B-32E1D120233F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{DD3696FE-717E-4025-B52C-339B2E8794CF}"/>
   </bookViews>
@@ -462,7 +462,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -502,8 +502,13 @@
         <f>B2</f>
         <v>6</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="D2" s="3">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3">
+        <f>C2-D2</f>
+        <v>2</v>
+      </c>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -518,7 +523,10 @@
         <v>5</v>
       </c>
       <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="E3" s="3">
+        <f t="shared" ref="E3:E8" si="1">C3-D3</f>
+        <v>5</v>
+      </c>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -533,7 +541,10 @@
         <v>12</v>
       </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="E4" s="3">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -548,7 +559,10 @@
         <v>15</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="E5" s="3">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -563,7 +577,10 @@
         <v>15</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="E6" s="3">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -578,7 +595,10 @@
         <v>10</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="E7" s="3">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -593,7 +613,10 @@
         <v>18</v>
       </c>
       <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="E8" s="3">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
       <c r="F8" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Person Constructor, Tasks chenged and some more stuff ...
</commit_message>
<xml_diff>
--- a/01_ProjectPlanning/Tasks/Tasks.xlsx
+++ b/01_ProjectPlanning/Tasks/Tasks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\SYP\if.05.61_01-project-repository\01_ProjectPlanning\Tasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D8DF41-02E5-44B4-AC8B-32E1D120233F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25E88E2-2AA8-4093-BB08-130D64D41384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{DD3696FE-717E-4025-B52C-339B2E8794CF}"/>
   </bookViews>
@@ -54,9 +54,6 @@
     <t>Responsible</t>
   </si>
   <si>
-    <t>Implement the virus with all ist math and physiks</t>
-  </si>
-  <si>
     <t>Rework all errors and get as close as possible to our desired output</t>
   </si>
   <si>
@@ -73,12 +70,18 @@
   </si>
   <si>
     <t>Implement calsses according to UML-class diagram without virus</t>
+  </si>
+  <si>
+    <t>Implement the virus with all its math and physiks</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -135,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -145,6 +148,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -462,7 +468,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -493,27 +499,26 @@
     </row>
     <row r="2" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3">
         <v>6</v>
       </c>
       <c r="C2" s="3">
-        <f>B2</f>
-        <v>6</v>
-      </c>
-      <c r="D2" s="3">
-        <v>4</v>
-      </c>
-      <c r="E2" s="3">
+        <v>8</v>
+      </c>
+      <c r="D2" s="5">
+        <v>5.5</v>
+      </c>
+      <c r="E2" s="5">
         <f>C2-D2</f>
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3">
         <v>5</v>
@@ -531,7 +536,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="3">
         <v>12</v>
@@ -549,7 +554,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3">
         <v>15</v>
@@ -567,7 +572,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="3">
         <v>15</v>
@@ -585,7 +590,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="3">
         <v>10</v>
@@ -603,7 +608,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="3">
         <v>18</v>

</xml_diff>

<commit_message>
Final commit before/after presentation and maybe the last? :(
</commit_message>
<xml_diff>
--- a/01_ProjectPlanning/Tasks/Tasks.xlsx
+++ b/01_ProjectPlanning/Tasks/Tasks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\SYP\if.05.61_01-project-repository\01_ProjectPlanning\Tasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F01CB9-4445-494B-A22D-06CDC7916D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA087AB-A2EE-4CD4-804E-616E77293345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{DD3696FE-717E-4025-B52C-339B2E8794CF}"/>
   </bookViews>
@@ -57,9 +57,6 @@
     <t>Rework all errors and get as close as possible to our desired output</t>
   </si>
   <si>
-    <t>If we got our desired output, we start with implemnting the rendererarrarereaere</t>
-  </si>
-  <si>
     <t>If were done with all we wanted and no changes have to be made anymore we start implementing another model to compare ours</t>
   </si>
   <si>
@@ -73,6 +70,9 @@
   </si>
   <si>
     <t>Implement classes according to UML-class diagram without virus</t>
+  </si>
+  <si>
+    <t>If we got our desired output, we start with implementing the view with the graphical output</t>
   </si>
 </sst>
 </file>
@@ -468,7 +468,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -499,7 +499,7 @@
     </row>
     <row r="2" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3">
         <v>18</v>
@@ -518,7 +518,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3">
         <v>15</v>
@@ -527,16 +527,18 @@
         <f t="shared" ref="C3:C8" si="0">B3</f>
         <v>15</v>
       </c>
-      <c r="D3" s="3"/>
+      <c r="D3" s="3">
+        <v>10</v>
+      </c>
       <c r="E3" s="3">
         <f t="shared" ref="E3:E8" si="1">C3-D3</f>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3">
         <v>36</v>
@@ -556,7 +558,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="3">
         <v>45</v>
@@ -585,34 +587,37 @@
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3">
+        <v>18</v>
+      </c>
       <c r="E6" s="3">
         <f t="shared" si="1"/>
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B7" s="3">
         <v>30</v>
       </c>
       <c r="C7" s="3">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="D7" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="D7" s="3">
+        <v>10</v>
+      </c>
       <c r="E7" s="3">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3">
         <v>54</v>
@@ -621,7 +626,9 @@
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="D8" s="3"/>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
       <c r="E8" s="3">
         <f t="shared" si="1"/>
         <v>54</v>

</xml_diff>